<commit_message>
Fixed mosfet logic, updated Regulator, Gerbers v4
</commit_message>
<xml_diff>
--- a/BSPD Part List.xlsx
+++ b/BSPD Part List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohit\Documents\Altium\Projects\Brake_System_Plausibility_Device\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohit\Documents\Altium\BSPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C9F597D-1814-407E-B0D2-90B34CFAB94B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F92E008-2AA8-4F61-8E39-691C9E019646}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{51207539-3F66-4F01-A872-DB023530BB28}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51207539-3F66-4F01-A872-DB023530BB28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>3 NOR GATE IC CHIP</t>
   </si>
   <si>
-    <t>L79L05ACUTR</t>
-  </si>
-  <si>
     <t>IC REG</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>C1206C105M4RACTU</t>
+  </si>
+  <si>
+    <t>MCP1703T-5003E/MB</t>
   </si>
 </sst>
 </file>
@@ -484,19 +484,19 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.46484375" customWidth="1"/>
-    <col min="2" max="2" width="25.46484375" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.59765625" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -518,18 +518,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -540,9 +540,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -551,7 +551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -573,20 +573,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -606,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -617,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -628,34 +628,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>61000821121</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -668,6 +668,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DF392E6CF0ECAD46A313F1F1AEA633DC" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0262b2c2c97ef7db4a11ebf68e26df9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f993596-de52-4d83-9dc9-85a2ec485321" xmlns:ns4="5af45bb2-5cac-4293-bf92-20dbf5d73737" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12e0513853f3d3c8927e1b46c024be01" ns3:_="" ns4:_="">
     <xsd:import namespace="8f993596-de52-4d83-9dc9-85a2ec485321"/>
@@ -852,15 +861,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -868,6 +868,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A055832E-EF5C-4910-A3DB-3F7EDA976994}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8963EEA9-4E3D-49D9-89F2-0FD0D7F928E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -886,14 +894,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A055832E-EF5C-4910-A3DB-3F7EDA976994}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D575F8E-45E4-4B3F-9107-BC52B04B8972}">
   <ds:schemaRefs>

</xml_diff>